<commit_message>
Final Push + Update ReadMe
Push all bugfixes, new tests and updated the readme file
</commit_message>
<xml_diff>
--- a/tests/Data Processing.xlsx
+++ b/tests/Data Processing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Makalah_Matdis\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5423D23-C8A5-4DCA-8899-515D279DB7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A76BBB-3605-4210-A349-A4F33BDC3845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{803EEE33-9123-4016-8516-FBF7EBF3962F}"/>
+    <workbookView minimized="1" xWindow="11220" yWindow="144" windowWidth="11820" windowHeight="8964" xr2:uid="{803EEE33-9123-4016-8516-FBF7EBF3962F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>Type</t>
   </si>
@@ -66,7 +66,13 @@
     <t>ISR</t>
   </si>
   <si>
-    <t>Time Per Pixel (ms)</t>
+    <t>Time Per Vector (ms)</t>
+  </si>
+  <si>
+    <t>Vectors</t>
+  </si>
+  <si>
+    <t>Difference (%)</t>
   </si>
 </sst>
 </file>
@@ -90,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -98,16 +104,239 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -259,10 +488,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$D$3:$D$5</c:f>
+              <c:f>Data!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4096</c:v>
                 </c:pt>
@@ -272,23 +501,35 @@
                 <c:pt idx="2">
                   <c:v>65536</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1048576</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$3:$H$5</c:f>
+              <c:f>Data!$I$3:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.36212801933288</c:v>
+                  <c:v>0.92756660779317202</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.638334433237667</c:v>
+                  <c:v>3.6917583147684669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.345994075139338</c:v>
+                  <c:v>15.028840859730968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.059371789296435</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>301.52211459477667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -542,7 +783,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$B$6</c:f>
+              <c:f>Data!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -619,10 +860,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$D$6:$D$8</c:f>
+              <c:f>Data!$D$8:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4096</c:v>
                 </c:pt>
@@ -632,23 +873,35 @@
                 <c:pt idx="2">
                   <c:v>65536</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1048576</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$6:$H$8</c:f>
+              <c:f>Data!$I$8:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.855879624684647</c:v>
+                  <c:v>1.0731099446614565</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.462353467941266</c:v>
+                  <c:v>4.1732235749562534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>133.21039239565465</c:v>
+                  <c:v>24.992307027180932</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.179062684377001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>341.181135574976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -922,7 +1175,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9247594050743664E-2"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.85333114610673666"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -976,6 +1239,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14409776902887139"/>
+                  <c:y val="0.12126239428404782"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1008,10 +1277,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$D$3:$D$5</c:f>
+              <c:f>Data!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4096</c:v>
                 </c:pt>
@@ -1021,23 +1290,35 @@
                 <c:pt idx="2">
                   <c:v>65536</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1048576</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$3:$H$5</c:f>
+              <c:f>Data!$I$3:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.36212801933288</c:v>
+                  <c:v>0.92756660779317202</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.638334433237667</c:v>
+                  <c:v>3.6917583147684669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.345994075139338</c:v>
+                  <c:v>15.028840859730968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.059371789296435</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>301.52211459477667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1054,7 +1335,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$B$6</c:f>
+              <c:f>Data!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1099,6 +1380,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.055511811023622E-2"/>
+                  <c:y val="-6.1902158063575387E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1131,10 +1418,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$D$6:$D$8</c:f>
+              <c:f>Data!$D$8:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4096</c:v>
                 </c:pt>
@@ -1144,23 +1431,35 @@
                 <c:pt idx="2">
                   <c:v>65536</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1048576</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$H$6:$H$8</c:f>
+              <c:f>Data!$I$8:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.855879624684647</c:v>
+                  <c:v>1.0731099446614565</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.462353467941266</c:v>
+                  <c:v>4.1732235749562534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>133.21039239565465</c:v>
+                  <c:v>24.992307027180932</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.179062684377001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>341.181135574976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1315,6 +1614,55 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.88802318460192475"/>
+          <c:y val="1.004556722076407E-2"/>
+          <c:w val="8.6976815398075238E-2"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3447,220 +3795,775 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAECEC2-3801-4707-BD33-8FE94FFDDE72}">
-  <dimension ref="B2:I8"/>
+  <dimension ref="B2:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>64</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <f>C3*C3</f>
         <v>4096</v>
       </c>
-      <c r="E3" s="2">
-        <v>3.2832832336425701</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3.3805069923400799</v>
-      </c>
-      <c r="G3" s="2">
-        <v>3.4225938320159899</v>
-      </c>
-      <c r="H3" s="2">
-        <f>AVERAGE(E3:G3)</f>
-        <v>3.36212801933288</v>
-      </c>
-      <c r="I3" s="2">
-        <f>H3/D3 * 1000</f>
-        <v>0.82083203596994136</v>
+      <c r="E3" s="1">
+        <f>D3+31</f>
+        <v>4127</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.905123710632324</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.93542098999023404</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.94215512275695801</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I12" si="0">AVERAGE(F3:H3)</f>
+        <v>0.92756660779317202</v>
+      </c>
+      <c r="J3" s="1">
+        <f>I3/E3 * 1000</f>
+        <v>0.22475565975119263</v>
+      </c>
+      <c r="K3">
+        <f>100 - J3/J8 * 100</f>
+        <v>13.56276098197938</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="17">
+        <v>4127</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0.92756660779317202</v>
+      </c>
+      <c r="P3" s="17">
+        <v>0.22475565975119263</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>13.56276098197938</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1">
         <v>128</v>
       </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4:D8" si="0">C4*C4</f>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D7" si="1">C4*C4</f>
         <v>16384</v>
       </c>
-      <c r="E4" s="2">
-        <v>14.088052272796601</v>
-      </c>
-      <c r="F4" s="2">
-        <v>13.3254923820495</v>
-      </c>
-      <c r="G4" s="2">
-        <v>13.501458644866901</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" ref="H4:H8" si="1">AVERAGE(E4:G4)</f>
-        <v>13.638334433237667</v>
-      </c>
-      <c r="I4" s="2">
-        <f t="shared" ref="I4:I8" si="2">H4/D4 * 1000</f>
-        <v>0.83241787312241622</v>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E12" si="2">D4+31</f>
+        <v>16415</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.5880503654479901</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3.77251720428466</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3.7147073745727499</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6917583147684669</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J12" si="3">I4/E4 * 1000</f>
+        <v>0.22490151171297393</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K7" si="4">100 - J4/J9 * 100</f>
+        <v>11.537010935073937</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="17">
+        <v>16415</v>
+      </c>
+      <c r="O4" s="6">
+        <v>3.6917583147684669</v>
+      </c>
+      <c r="P4" s="17">
+        <v>0.22490151171297393</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>11.537010935073937</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1">
         <v>256</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>65567</v>
+      </c>
+      <c r="F5" s="1">
+        <v>14.4278225898742</v>
+      </c>
+      <c r="G5" s="1">
+        <v>14.958247423171899</v>
+      </c>
+      <c r="H5" s="1">
+        <v>15.700452566146801</v>
+      </c>
+      <c r="I5" s="1">
         <f t="shared" si="0"/>
+        <v>15.028840859730968</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.22921348940367819</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>39.866132232666551</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="17">
+        <v>65567</v>
+      </c>
+      <c r="O5" s="6">
+        <v>15.028840859730968</v>
+      </c>
+      <c r="P5" s="17">
+        <v>0.22921348940367819</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>39.866132232666551</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1">
+        <v>512</v>
+      </c>
+      <c r="D6" s="1">
+        <f>C6*C6</f>
+        <v>262144</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>262175</v>
+      </c>
+      <c r="F6" s="1">
+        <v>66.548743724822998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>69.823835134506197</v>
+      </c>
+      <c r="H6" s="1">
+        <v>67.805536508560095</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>68.059371789296435</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25959520087459304</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>22.81685729309217</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="17">
+        <v>262175</v>
+      </c>
+      <c r="O6" s="6">
+        <v>68.059371789296435</v>
+      </c>
+      <c r="P6" s="17">
+        <v>0.25959520087459304</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>22.81685729309217</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>1048576</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>1048607</v>
+      </c>
+      <c r="F7" s="1">
+        <v>300.63607764244</v>
+      </c>
+      <c r="G7" s="1">
+        <v>299.56093168258599</v>
+      </c>
+      <c r="H7" s="1">
+        <v>304.36933445930401</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>301.52211459477667</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.28754539555312592</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>11.624036866330215</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="17">
+        <v>1048607</v>
+      </c>
+      <c r="O7" s="6">
+        <v>301.52211459477667</v>
+      </c>
+      <c r="P7" s="17">
+        <v>0.28754539555312592</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>11.624036866330215</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1">
+        <f>C8*C8</f>
+        <v>4096</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>4127</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.0709199905395499</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.0902836322784399</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.0581262111663801</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0731099446614565</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.26002179419952909</v>
+      </c>
+      <c r="K8">
+        <f>J8/J3 *100 - 100</f>
+        <v>15.690877145152427</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="11">
+        <v>4127</v>
+      </c>
+      <c r="O8" s="3">
+        <v>1.0731099446614565</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0.26002179419952909</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>15.690877145152427</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1">
+        <v>128</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" ref="D9:D12" si="5">C9*C9</f>
+        <v>16384</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>16415</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.1586270332336399</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4.3012087345123202</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.0598349571228001</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1732235749562534</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25423232256815431</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K12" si="6">J9/J4 *100 - 100</f>
+        <v>13.041624590150917</v>
+      </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="17">
+        <v>16415</v>
+      </c>
+      <c r="O9" s="6">
+        <v>4.1732235749562534</v>
+      </c>
+      <c r="P9" s="17">
+        <v>0.25423232256815431</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>13.041624590150917</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1">
+        <v>256</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="5"/>
         <v>65536</v>
       </c>
-      <c r="E5" s="2">
-        <v>48.078533172607401</v>
-      </c>
-      <c r="F5" s="2">
-        <v>50.868062257766702</v>
-      </c>
-      <c r="G5" s="2">
-        <v>55.091386795043903</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" si="1"/>
-        <v>51.345994075139338</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>0.78347769279692592</v>
+        <v>65567</v>
+      </c>
+      <c r="F10" s="1">
+        <v>25.003004550933799</v>
+      </c>
+      <c r="G10" s="1">
+        <v>25.9727685451507</v>
+      </c>
+      <c r="H10" s="1">
+        <v>24.001147985458299</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>24.992307027180932</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.38117203817745104</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
+        <v>66.295639566898188</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="17">
+        <v>65567</v>
+      </c>
+      <c r="O10" s="6">
+        <v>24.992307027180932</v>
+      </c>
+      <c r="P10" s="17">
+        <v>0.38117203817745104</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>66.295639566898188</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1">
+        <v>512</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="5"/>
+        <v>262144</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>262175</v>
+      </c>
+      <c r="F11" s="1">
+        <v>88.643239498138399</v>
+      </c>
+      <c r="G11" s="1">
+        <v>89.817884683608995</v>
+      </c>
+      <c r="H11" s="1">
+        <v>86.076063871383596</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>88.179062684377001</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.33633665560933351</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>29.56196974219614</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="17">
+        <v>262175</v>
+      </c>
+      <c r="O11" s="6">
+        <v>88.179062684377001</v>
+      </c>
+      <c r="P11" s="17">
+        <v>0.33633665560933351</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>29.56196974219614</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="5"/>
+        <v>1048576</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>1048607</v>
+      </c>
+      <c r="F12" s="1">
+        <v>336.95704579353298</v>
+      </c>
+      <c r="G12" s="1">
+        <v>337.82286405563298</v>
+      </c>
+      <c r="H12" s="1">
+        <v>348.76349687576197</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>341.181135574976</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.32536606714906152</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>13.152939390033808</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="18">
+        <v>1048607</v>
+      </c>
+      <c r="O12" s="9">
+        <v>341.181135574976</v>
+      </c>
+      <c r="P12" s="18">
+        <v>0.32536606714906152</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>13.152939390033808</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6">
+        <v>64</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0.905123710632324</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.93542098999023404</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.94215512275695801</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0.92756660779317202</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="6">
+        <v>128</v>
+      </c>
+      <c r="D16" s="17">
+        <v>3.5880503654479901</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3.77251720428466</v>
+      </c>
+      <c r="F16" s="17">
+        <v>3.7147073745727499</v>
+      </c>
+      <c r="G16" s="17">
+        <v>3.6917583147684669</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="6">
+        <v>256</v>
+      </c>
+      <c r="D17" s="17">
+        <v>14.4278225898742</v>
+      </c>
+      <c r="E17" s="6">
+        <v>14.958247423171899</v>
+      </c>
+      <c r="F17" s="17">
+        <v>15.700452566146801</v>
+      </c>
+      <c r="G17" s="17">
+        <v>15.028840859730968</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="6">
+        <v>512</v>
+      </c>
+      <c r="D18" s="17">
+        <v>66.548743724822998</v>
+      </c>
+      <c r="E18" s="6">
+        <v>69.823835134506197</v>
+      </c>
+      <c r="F18" s="17">
+        <v>67.805536508560095</v>
+      </c>
+      <c r="G18" s="17">
+        <v>68.059371789296435</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="13"/>
+      <c r="C19" s="9">
+        <v>1024</v>
+      </c>
+      <c r="D19" s="18">
+        <v>300.63607764244</v>
+      </c>
+      <c r="E19" s="9">
+        <v>299.56093168258599</v>
+      </c>
+      <c r="F19" s="18">
+        <v>304.36933445930401</v>
+      </c>
+      <c r="G19" s="18">
+        <v>301.52211459477667</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C20" s="6">
         <v>64</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>4096</v>
-      </c>
-      <c r="E6" s="2">
-        <v>7.8021726608276296</v>
-      </c>
-      <c r="F6" s="2">
-        <v>7.8718233108520499</v>
-      </c>
-      <c r="G6" s="2">
-        <v>7.8936429023742596</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="1"/>
-        <v>7.855879624684647</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="2"/>
-        <v>1.9179393614952751</v>
+      <c r="D20" s="17">
+        <v>1.0709199905395499</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.0902836322784399</v>
+      </c>
+      <c r="F20" s="17">
+        <v>1.0581262111663801</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1.0731099446614565</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="6">
         <v>128</v>
       </c>
-      <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>16384</v>
-      </c>
-      <c r="E7" s="2">
-        <v>32.654962778091402</v>
-      </c>
-      <c r="F7" s="2">
-        <v>31.0308871269226</v>
-      </c>
-      <c r="G7" s="2">
-        <v>30.7012104988098</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="1"/>
-        <v>31.462353467941266</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="2"/>
-        <v>1.9203096599085245</v>
+      <c r="D21" s="17">
+        <v>4.1586270332336399</v>
+      </c>
+      <c r="E21" s="6">
+        <v>4.3012087345123202</v>
+      </c>
+      <c r="F21" s="17">
+        <v>4.0598349571228001</v>
+      </c>
+      <c r="G21" s="17">
+        <v>4.1732235749562534</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="6">
         <v>256</v>
       </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>65536</v>
-      </c>
-      <c r="E8" s="2">
-        <v>128.790952444076</v>
-      </c>
-      <c r="F8" s="2">
-        <v>137.07436847686699</v>
-      </c>
-      <c r="G8" s="2">
-        <v>133.76585626602099</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" si="1"/>
-        <v>133.21039239565465</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="2"/>
-        <v>2.0326292784981486</v>
+      <c r="D22" s="17">
+        <v>25.003004550933799</v>
+      </c>
+      <c r="E22" s="6">
+        <v>25.9727685451507</v>
+      </c>
+      <c r="F22" s="17">
+        <v>24.001147985458299</v>
+      </c>
+      <c r="G22" s="17">
+        <v>24.992307027180932</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="6">
+        <v>512</v>
+      </c>
+      <c r="D23" s="17">
+        <v>88.643239498138399</v>
+      </c>
+      <c r="E23" s="6">
+        <v>89.817884683608995</v>
+      </c>
+      <c r="F23" s="17">
+        <v>86.076063871383596</v>
+      </c>
+      <c r="G23" s="17">
+        <v>88.179062684377001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="13"/>
+      <c r="C24" s="9">
+        <v>1024</v>
+      </c>
+      <c r="D24" s="18">
+        <v>336.95704579353298</v>
+      </c>
+      <c r="E24" s="9">
+        <v>337.82286405563298</v>
+      </c>
+      <c r="F24" s="18">
+        <v>348.76349687576197</v>
+      </c>
+      <c r="G24" s="18">
+        <v>341.181135574976</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
+  <mergeCells count="6">
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="M8:M12"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B15:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3686,7 +4589,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3700,8 +4603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B757555-424D-40F4-B03A-55FADAF9FA15}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>